<commit_message>
edited .csv to Results.xlsx
test
</commit_message>
<xml_diff>
--- a/UploadTemplatetest.xlsx
+++ b/UploadTemplatetest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77E050AE-773B-4C35-A6AF-5FFDF87598C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C42D54E5-49E4-4B68-B76B-D88F3361198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -777,7 +777,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,7 +895,7 @@
   <dimension ref="A1:Q500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,19 +981,19 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C25" ca="1" si="0">4*MAX(0,ROUND(NORMINV(RAND(),1236,365),0))</f>
-        <v>5552</v>
+        <v>5264</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D25" ca="1" si="1">4*MAX(0,ROUND(NORMINV(RAND(),745,365),0))</f>
-        <v>2824</v>
+        <v>3444</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E25" ca="1" si="2">4*MAX(0,ROUND(NORMINV(RAND(),586,163),0))</f>
-        <v>2452</v>
+        <v>2072</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F25" ca="1" si="3">4*MAX(0,ROUND(NORMINV(RAND(),189,50),0))</f>
-        <v>584</v>
+        <v>772</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -1003,19 +1003,19 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>6516</v>
+        <v>6040</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1264</v>
+        <v>3496</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="2"/>
-        <v>3284</v>
+        <v>2656</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="3"/>
-        <v>916</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -1025,19 +1025,19 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6936</v>
+        <v>4956</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3812</v>
+        <v>4840</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>1840</v>
+        <v>1836</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="3"/>
-        <v>768</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -1047,19 +1047,19 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>3600</v>
+        <v>4812</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>2352</v>
+        <v>3904</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>1712</v>
+        <v>1852</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="3"/>
-        <v>836</v>
+        <v>728</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -1069,19 +1069,19 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>3448</v>
+        <v>3720</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1552</v>
+        <v>960</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>2708</v>
+        <v>2060</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
-        <v>688</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1091,19 +1091,19 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>4892</v>
+        <v>5144</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>2960</v>
+        <v>3308</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>2600</v>
+        <v>3036</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>396</v>
+        <v>784</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
@@ -1113,19 +1113,19 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>6140</v>
+        <v>3476</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>3332</v>
+        <v>4784</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>3008</v>
+        <v>3148</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>944</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -1134,19 +1134,19 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>6660</v>
+        <v>5108</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>1112</v>
+        <v>2128</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>692</v>
+        <v>712</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -1155,19 +1155,19 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>2036</v>
+        <v>5140</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>1636</v>
+        <v>2728</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>2580</v>
+        <v>3124</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>448</v>
+        <v>596</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -1176,19 +1176,19 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>3808</v>
+        <v>7124</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>644</v>
+        <v>4232</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>2632</v>
+        <v>2520</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>192</v>
+        <v>620</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -1197,19 +1197,19 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>7068</v>
+        <v>4456</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>3976</v>
+        <v>3608</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>1788</v>
+        <v>2888</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
-        <v>696</v>
+        <v>960</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
@@ -1218,19 +1218,19 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>2860</v>
+        <v>4932</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>1300</v>
+        <v>1800</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>2936</v>
+        <v>2716</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="3"/>
-        <v>1116</v>
+        <v>900</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -1239,19 +1239,19 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>4820</v>
+        <v>6200</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>4664</v>
+        <v>3336</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>2184</v>
+        <v>1760</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="3"/>
-        <v>868</v>
+        <v>876</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -1260,19 +1260,19 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>2052</v>
+        <v>7844</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>3916</v>
+        <v>2056</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>1864</v>
+        <v>2144</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="3"/>
-        <v>760</v>
+        <v>844</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -1281,19 +1281,19 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>3116</v>
+        <v>4216</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>4568</v>
+        <v>5444</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>2992</v>
+        <v>2392</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="3"/>
-        <v>568</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -1302,19 +1302,19 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>2136</v>
+        <v>5656</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>3216</v>
+        <v>3808</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>1948</v>
+        <v>1924</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="3"/>
-        <v>744</v>
+        <v>952</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
@@ -1323,19 +1323,19 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>5472</v>
+        <v>4452</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>4228</v>
+        <v>3844</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>1956</v>
+        <v>1816</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="3"/>
-        <v>840</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
@@ -1344,19 +1344,19 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>3456</v>
+        <v>6160</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4324</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>1944</v>
+        <v>2484</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="3"/>
-        <v>1100</v>
+        <v>748</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
@@ -1365,19 +1365,19 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>4048</v>
+        <v>2508</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>2668</v>
+        <v>3920</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>3856</v>
+        <v>2520</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="3"/>
-        <v>492</v>
+        <v>660</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
@@ -1386,19 +1386,19 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>4404</v>
+        <v>5564</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>4596</v>
+        <v>4136</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>2640</v>
+        <v>1964</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="3"/>
-        <v>720</v>
+        <v>572</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
@@ -1407,19 +1407,19 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>5344</v>
+        <v>5860</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>1516</v>
+        <v>1544</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>1024</v>
+        <v>1588</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="3"/>
-        <v>1144</v>
+        <v>608</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
@@ -1428,19 +1428,19 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>3096</v>
+        <v>3456</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>3560</v>
+        <v>1484</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>2808</v>
+        <v>1836</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="3"/>
-        <v>744</v>
+        <v>640</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
@@ -1449,19 +1449,19 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>5716</v>
+        <v>6388</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>2288</v>
+        <v>1700</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>3372</v>
+        <v>1164</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="3"/>
-        <v>916</v>
+        <v>848</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
@@ -1470,19 +1470,19 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>6556</v>
+        <v>5276</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>2812</v>
+        <v>4220</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>3488</v>
+        <v>2296</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="3"/>
-        <v>188</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
@@ -3867,19 +3867,19 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C25" ca="1" si="0">4*MAX(0,ROUND(NORMINV(RAND(),1236,365),0))</f>
-        <v>4748</v>
+        <v>5540</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D25" ca="1" si="1">4*MAX(0,ROUND(NORMINV(RAND(),745,365),0))</f>
-        <v>2368</v>
+        <v>1940</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E25" ca="1" si="2">4*MAX(0,ROUND(NORMINV(RAND(),586,163),0))</f>
-        <v>1780</v>
+        <v>2164</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F25" ca="1" si="3">4*MAX(0,ROUND(NORMINV(RAND(),189,50),0))</f>
-        <v>976</v>
+        <v>832</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -3889,19 +3889,19 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>6324</v>
+        <v>3520</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1628</v>
+        <v>4744</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="2"/>
-        <v>1756</v>
+        <v>3268</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="3"/>
-        <v>876</v>
+        <v>932</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -3911,19 +3911,19 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>8932</v>
+        <v>2324</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>2540</v>
+        <v>4980</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>2120</v>
+        <v>1992</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="3"/>
-        <v>696</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -3933,19 +3933,19 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>2892</v>
+        <v>5340</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>908</v>
+        <v>4964</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>2992</v>
+        <v>2344</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="3"/>
-        <v>532</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -3955,19 +3955,19 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>4608</v>
+        <v>6848</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>4216</v>
+        <v>2312</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>2304</v>
+        <v>1892</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
-        <v>724</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3977,19 +3977,19 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>1424</v>
+        <v>4056</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>3424</v>
+        <v>1516</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>1844</v>
+        <v>1648</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>812</v>
+        <v>880</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
@@ -3999,19 +3999,19 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>3596</v>
+        <v>5380</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>2068</v>
+        <v>412</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>2872</v>
+        <v>1324</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>856</v>
+        <v>788</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -4020,19 +4020,19 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>4568</v>
+        <v>3448</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>3624</v>
+        <v>3116</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>2388</v>
+        <v>1032</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>408</v>
+        <v>812</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -4041,19 +4041,19 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>4712</v>
+        <v>4884</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>2680</v>
+        <v>2660</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>976</v>
+        <v>3076</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>840</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -4062,19 +4062,19 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>4868</v>
+        <v>6688</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>4456</v>
+        <v>4628</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>2596</v>
+        <v>1276</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>348</v>
+        <v>692</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -4083,19 +4083,19 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>3680</v>
+        <v>6012</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>1680</v>
+        <v>800</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>3256</v>
+        <v>2476</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
-        <v>892</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
@@ -4104,19 +4104,19 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>5868</v>
+        <v>3592</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>3184</v>
+        <v>4052</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>3056</v>
+        <v>1812</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="3"/>
-        <v>1040</v>
+        <v>724</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -4125,19 +4125,19 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>5536</v>
+        <v>4756</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>3696</v>
+        <v>3768</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>2016</v>
+        <v>1568</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="3"/>
-        <v>580</v>
+        <v>856</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -4146,19 +4146,19 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>3208</v>
+        <v>4284</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>5720</v>
+        <v>1096</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>1940</v>
+        <v>2496</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="3"/>
-        <v>516</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -4167,19 +4167,19 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>6992</v>
+        <v>6488</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>3556</v>
+        <v>912</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>2968</v>
+        <v>2420</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="3"/>
-        <v>780</v>
+        <v>652</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -4188,19 +4188,19 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>4880</v>
+        <v>3944</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>3524</v>
+        <v>2228</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>2720</v>
+        <v>1768</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="3"/>
-        <v>964</v>
+        <v>768</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
@@ -4209,19 +4209,19 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>4268</v>
+        <v>3148</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>2528</v>
+        <v>2676</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>1744</v>
+        <v>3284</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="3"/>
-        <v>644</v>
+        <v>884</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
@@ -4230,19 +4230,19 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>3852</v>
+        <v>8056</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>5868</v>
+        <v>5008</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>2952</v>
+        <v>2756</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="3"/>
-        <v>1036</v>
+        <v>880</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
@@ -4251,19 +4251,19 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>3828</v>
+        <v>3016</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>728</v>
+        <v>3824</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>1176</v>
+        <v>2972</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="3"/>
-        <v>840</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
@@ -4272,19 +4272,19 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>2116</v>
+        <v>4996</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>2240</v>
+        <v>3496</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>2404</v>
+        <v>2444</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="3"/>
-        <v>740</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
@@ -4293,19 +4293,19 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>4788</v>
+        <v>6300</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>2756</v>
+        <v>4036</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>1192</v>
+        <v>2772</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="3"/>
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
@@ -4314,19 +4314,19 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>5356</v>
+        <v>5792</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>5040</v>
+        <v>3236</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>2648</v>
+        <v>2952</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="3"/>
-        <v>760</v>
+        <v>696</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
@@ -4335,19 +4335,19 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>5556</v>
+        <v>4984</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>3432</v>
+        <v>1648</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>2660</v>
+        <v>2600</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="3"/>
-        <v>736</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
@@ -4356,19 +4356,19 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>5080</v>
+        <v>3420</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>5108</v>
+        <v>3916</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>1904</v>
+        <v>1492</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="3"/>
-        <v>912</v>
+        <v>844</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">

</xml_diff>